<commit_message>
desafio 5 update v1
</commit_message>
<xml_diff>
--- a/Desafio5/Inputs/Lista_de_Materiais_de_Escritorio.xlsx
+++ b/Desafio5/Inputs/Lista_de_Materiais_de_Escritorio.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomationEdge\Desafios\Desafio5\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B9EF870-4F48-4EBF-9476-D6B2A9501551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A71E489-8DBC-4201-A1B8-F3ED4BCEB6F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{BE0D0478-BDA1-426E-A60A-AEB12FD17448}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" activeTab="1" xr2:uid="{BE0D0478-BDA1-426E-A60A-AEB12FD17448}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$E$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$C$28</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="88">
   <si>
     <t>Descrição</t>
   </si>
@@ -252,6 +253,57 @@
   </si>
   <si>
     <t>//*[@id="product-info"]/div/section[2]/div[2]/div[2]/div/div[3]/div[1]/div[2]/div[1]/span[3]/span[2]</t>
+  </si>
+  <si>
+    <t>//*[@data-testid="heading-product-title"]</t>
+  </si>
+  <si>
+    <t>//*[@data-testid="price-value"]</t>
+  </si>
+  <si>
+    <t>//*[@id="rsyswpsdk"]/div/main/div[3]/div[2]/div[1]/div[2]/div</t>
+  </si>
+  <si>
+    <t>//*[@id="shopify-section-product-template"]/div[1]/h1</t>
+  </si>
+  <si>
+    <t>//*[@class="preco_a_vista"]</t>
+  </si>
+  <si>
+    <t>//*[@id="product-top"]/div[3]/h1</t>
+  </si>
+  <si>
+    <t>//*[@id="product-top"]/div[5]/div[2]/div[2]/div[1]/div/span[2]</t>
+  </si>
+  <si>
+    <t>//*[@id="product-price"]</t>
+  </si>
+  <si>
+    <t>//*[@id="product-wrapper"]/div[1]/div[2]/h1</t>
+  </si>
+  <si>
+    <t>//*[@id="rsyswpsdk"]/div/main/div[2]/div[1]/div[2]/h1</t>
+  </si>
+  <si>
+    <t>//*[@id="rsyswpsdk"]/div/main/div[2]/div[2]/div[1]/div[1]/div</t>
+  </si>
+  <si>
+    <t>//*[@id="__next"]/div/div[2]/div[2]/div[2]/div[2]/div/div/div/h1</t>
+  </si>
+  <si>
+    <t>//*[@id="variacaoPreco"]</t>
+  </si>
+  <si>
+    <t>//*[@class="dsvia-heading css-1xmpwke"]</t>
+  </si>
+  <si>
+    <t>//h1[@class="vtex-store-components-3-x-productNameContainer mv0 t-heading-4"]</t>
+  </si>
+  <si>
+    <t>//div[contains(@class,'flex-column items-start flex')]</t>
+  </si>
+  <si>
+    <t>//*[@class="product-title__Title-sc-15fh86r-0 iYwPCy"]</t>
   </si>
 </sst>
 </file>
@@ -261,7 +313,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -273,12 +325,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -306,7 +352,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -314,19 +360,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -642,346 +707,492 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C624A2B-C953-4D28-AB60-675AC9316AA8}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="52.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="93.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="255.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="C2" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="C3" s="6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="C4" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="C5" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="C6" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="C7" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="C8" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="C9" s="7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="C10" s="7" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="C11" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E12" t="s">
+      <c r="C12" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E13" t="s">
+      <c r="C13" s="8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E14" t="s">
+      <c r="C14" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E15" t="s">
+      <c r="C15" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E16" t="s">
+      <c r="C16" s="8" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E17" t="s">
+      <c r="C17" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E18" t="s">
+      <c r="C18" s="8" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E19" t="s">
+      <c r="C19" s="8" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E20" t="s">
+      <c r="C20" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E21" t="s">
+      <c r="C21" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E22" t="s">
+      <c r="C22" s="8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E23" t="s">
+      <c r="C23" s="8" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E24" t="s">
+      <c r="C24" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E25" t="s">
+      <c r="C25" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E26" t="s">
+      <c r="C26" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E27" t="s">
+      <c r="C27" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E28" t="s">
+      <c r="C28" s="8" t="s">
         <v>58</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{74BA4D15-248A-449D-9B47-71DDED94BAA1}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{74BA4D15-248A-449D-9B47-71DDED94BAA1}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{95E2A144-8BF3-4847-8F18-33A706A8AF31}"/>
+    <hyperlink ref="C5" r:id="rId3" xr:uid="{ACA07146-C8BD-454B-BA1C-B09D678D08A1}"/>
+    <hyperlink ref="C6" r:id="rId4" xr:uid="{60CFD895-9722-49A6-90C6-CFBE0CC3C1B6}"/>
+    <hyperlink ref="C7" r:id="rId5" xr:uid="{B99EE206-5157-48D9-A010-A068985F275B}"/>
+    <hyperlink ref="C12" r:id="rId6" xr:uid="{16A7ED72-EA73-48B8-AC20-853455E67C4B}"/>
+    <hyperlink ref="C19" r:id="rId7" xr:uid="{7FF9C3CE-D8D8-4DDA-91F8-B49D65F32B7C}"/>
+    <hyperlink ref="C16" r:id="rId8" xr:uid="{2D463425-CE10-4054-A1BC-9F4A0BCCE347}"/>
+    <hyperlink ref="C28" r:id="rId9" display="https://www.submarino.com.br/produto/1698410107?pfm_carac=cadeira-giratoria-para-escritorio&amp;pfm_index=1&amp;pfm_page=search&amp;pfm_pos=grid&amp;pfm_type=search_page&amp;offerId=5eb5ac7879bf8430cb3f3233&amp;chave=b2wads_61156641117c9d001601fc28_20682612000119_1698410107_77c91966-1650-450e-958b-cde99d0b7cf2" xr:uid="{004FCDCB-DCF7-45BE-BF4F-94147F0A1D17}"/>
+    <hyperlink ref="C26" r:id="rId10" xr:uid="{A3CE471E-5F86-409A-AD1D-2215DB86ACA1}"/>
+    <hyperlink ref="C23" r:id="rId11" xr:uid="{C616D098-58F7-4CB8-ABA2-34056012A10B}"/>
+    <hyperlink ref="C8" r:id="rId12" xr:uid="{0CDE6611-2825-4689-A08C-BAC1B99445AB}"/>
+    <hyperlink ref="C22" r:id="rId13" xr:uid="{BF76DC7E-E58A-45DE-A521-2E325538798C}"/>
+    <hyperlink ref="C4" r:id="rId14" xr:uid="{8CA1854B-8194-43EE-89E8-626A3F4F1C5D}"/>
+    <hyperlink ref="C11" r:id="rId15" xr:uid="{E24AC9E8-E0CA-4F37-9A75-A647953D276B}"/>
+    <hyperlink ref="C18" r:id="rId16" xr:uid="{85FC708C-2495-4DEA-9D3F-649CE5786485}"/>
+    <hyperlink ref="C13" r:id="rId17" xr:uid="{0E6FEA31-0715-40A2-9703-A77D3D1136D9}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId18"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59A0940F-6E72-4A99-9E15-3DDE394309D7}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="78" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="93.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C11">
+    <sortCondition ref="A2:A11"/>
+  </sortState>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>